<commit_message>
proof of f(a, d, f) monotonicity
</commit_message>
<xml_diff>
--- a/profiles/omnibus-checkfile-working.xlsx
+++ b/profiles/omnibus-checkfile-working.xlsx
@@ -211,15 +211,16 @@
   <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="2" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="6.75"/>
-    <col collapsed="false" hidden="false" max="17" min="8" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="6" min="2" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="17" min="8" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -953,67 +954,67 @@
       </c>
       <c r="B12" s="0" t="n">
         <f aca="false">0.05*B17+0.07*B18</f>
-        <v>1070</v>
+        <v>1000</v>
       </c>
       <c r="C12" s="0" t="n">
         <f aca="false">0.05*C17+0.07*C18</f>
-        <v>1140</v>
+        <v>1000</v>
       </c>
       <c r="D12" s="0" t="n">
         <f aca="false">0.05*D17+0.07*D18</f>
-        <v>1210</v>
+        <v>1000</v>
       </c>
       <c r="E12" s="0" t="n">
         <f aca="false">0.05*E17+0.07*E18</f>
-        <v>1280</v>
+        <v>1000</v>
       </c>
       <c r="F12" s="0" t="n">
         <f aca="false">0.05*F17+0.07*F18</f>
-        <v>1350</v>
+        <v>1000</v>
       </c>
       <c r="G12" s="1" t="n">
         <f aca="false">0.05*G17+0.07*G18</f>
-        <v>1420</v>
+        <v>1000</v>
       </c>
       <c r="H12" s="0" t="n">
         <f aca="false">0.05*H17+0.07*H18</f>
-        <v>1420</v>
+        <v>1000</v>
       </c>
       <c r="I12" s="0" t="n">
         <f aca="false">0.05*I17+0.07*I18</f>
-        <v>1420</v>
+        <v>1000</v>
       </c>
       <c r="J12" s="0" t="n">
         <f aca="false">0.05*J17+0.07*J18</f>
-        <v>1420</v>
+        <v>1000</v>
       </c>
       <c r="K12" s="0" t="n">
         <f aca="false">0.05*K17+0.07*K18</f>
-        <v>1420</v>
+        <v>1000</v>
       </c>
       <c r="L12" s="0" t="n">
         <f aca="false">0.05*L17+0.07*L18</f>
-        <v>1420</v>
+        <v>1000</v>
       </c>
       <c r="M12" s="0" t="n">
         <f aca="false">0.05*M17+0.07*M18</f>
-        <v>1420</v>
+        <v>1000</v>
       </c>
       <c r="N12" s="0" t="n">
         <f aca="false">0.05*N17+0.07*N18</f>
-        <v>1420</v>
+        <v>1000</v>
       </c>
       <c r="O12" s="0" t="n">
         <f aca="false">0.05*O17+0.07*O18</f>
-        <v>1420</v>
+        <v>1000</v>
       </c>
       <c r="P12" s="0" t="n">
         <f aca="false">0.05*P17+0.07*P18</f>
-        <v>1420</v>
+        <v>1000</v>
       </c>
       <c r="Q12" s="0" t="n">
         <f aca="false">0.05*Q17+0.07*Q18</f>
-        <v>1420</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1022,67 +1023,67 @@
       </c>
       <c r="B13" s="0" t="n">
         <f aca="false">B10+B11-B12</f>
-        <v>3016</v>
+        <v>3086</v>
       </c>
       <c r="C13" s="0" t="n">
         <f aca="false">C10+C11-C12</f>
-        <v>2946</v>
+        <v>3086</v>
       </c>
       <c r="D13" s="0" t="n">
         <f aca="false">D10+D11-D12</f>
-        <v>2876</v>
+        <v>3086</v>
       </c>
       <c r="E13" s="0" t="n">
         <f aca="false">E10+E11-E12</f>
-        <v>2806</v>
+        <v>3086</v>
       </c>
       <c r="F13" s="0" t="n">
         <f aca="false">F10+F11-F12</f>
-        <v>2736</v>
+        <v>3086</v>
       </c>
       <c r="G13" s="1" t="n">
         <f aca="false">G10+G11-G12</f>
-        <v>2666</v>
+        <v>3086</v>
       </c>
       <c r="H13" s="0" t="n">
         <f aca="false">H10+H11-H12</f>
-        <v>2760.176</v>
+        <v>3180.176</v>
       </c>
       <c r="I13" s="0" t="n">
         <f aca="false">I10+I11-I12</f>
-        <v>2855.858816</v>
+        <v>3275.858816</v>
       </c>
       <c r="J13" s="0" t="n">
         <f aca="false">J10+J11-J12</f>
-        <v>2953.072557056</v>
+        <v>3373.072557056</v>
       </c>
       <c r="K13" s="0" t="n">
         <f aca="false">K10+K11-K12</f>
-        <v>3051.8417179689</v>
+        <v>3471.8417179689</v>
       </c>
       <c r="L13" s="0" t="n">
         <f aca="false">L10+L11-L12</f>
-        <v>3152.1911854564</v>
+        <v>3572.1911854564</v>
       </c>
       <c r="M13" s="0" t="n">
         <f aca="false">M10+M11-M12</f>
-        <v>3254.1462444237</v>
+        <v>3674.1462444237</v>
       </c>
       <c r="N13" s="0" t="n">
         <f aca="false">N10+N11-N12</f>
-        <v>3357.73258433448</v>
+        <v>3777.73258433448</v>
       </c>
       <c r="O13" s="0" t="n">
         <f aca="false">O10+O11-O12</f>
-        <v>3462.97630568383</v>
+        <v>3882.97630568383</v>
       </c>
       <c r="P13" s="0" t="n">
         <f aca="false">P10+P11-P12</f>
-        <v>3569.90392657477</v>
+        <v>3989.90392657477</v>
       </c>
       <c r="Q13" s="0" t="n">
         <f aca="false">Q10+Q11-Q12</f>
-        <v>3678.54238939997</v>
+        <v>4098.54238939997</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1091,67 +1092,67 @@
       </c>
       <c r="B14" s="0" t="n">
         <f aca="false">0.335*B13</f>
-        <v>1010.36</v>
+        <v>1033.81</v>
       </c>
       <c r="C14" s="0" t="n">
         <f aca="false">0.335*C13</f>
-        <v>986.91</v>
+        <v>1033.81</v>
       </c>
       <c r="D14" s="0" t="n">
         <f aca="false">0.335*D13</f>
-        <v>963.46</v>
+        <v>1033.81</v>
       </c>
       <c r="E14" s="0" t="n">
         <f aca="false">0.335*E13</f>
-        <v>940.01</v>
+        <v>1033.81</v>
       </c>
       <c r="F14" s="0" t="n">
         <f aca="false">0.335*F13</f>
-        <v>916.56</v>
+        <v>1033.81</v>
       </c>
       <c r="G14" s="1" t="n">
         <f aca="false">0.335*G13</f>
-        <v>893.11</v>
+        <v>1033.81</v>
       </c>
       <c r="H14" s="0" t="n">
         <f aca="false">0.335*H13</f>
-        <v>924.65896</v>
+        <v>1065.35896</v>
       </c>
       <c r="I14" s="0" t="n">
         <f aca="false">0.335*I13</f>
-        <v>956.71270336</v>
+        <v>1097.41270336</v>
       </c>
       <c r="J14" s="0" t="n">
         <f aca="false">0.335*J13</f>
-        <v>989.27930661376</v>
+        <v>1129.97930661376</v>
       </c>
       <c r="K14" s="0" t="n">
         <f aca="false">0.335*K13</f>
-        <v>1022.36697551958</v>
+        <v>1163.06697551958</v>
       </c>
       <c r="L14" s="0" t="n">
         <f aca="false">0.335*L13</f>
-        <v>1055.98404712789</v>
+        <v>1196.68404712789</v>
       </c>
       <c r="M14" s="0" t="n">
         <f aca="false">0.335*M13</f>
-        <v>1090.13899188194</v>
+        <v>1230.83899188194</v>
       </c>
       <c r="N14" s="0" t="n">
         <f aca="false">0.335*N13</f>
-        <v>1124.84041575205</v>
+        <v>1265.54041575205</v>
       </c>
       <c r="O14" s="0" t="n">
         <f aca="false">0.335*O13</f>
-        <v>1160.09706240408</v>
+        <v>1300.79706240408</v>
       </c>
       <c r="P14" s="0" t="n">
         <f aca="false">0.335*P13</f>
-        <v>1195.91781540255</v>
+        <v>1336.61781540255</v>
       </c>
       <c r="Q14" s="0" t="n">
         <f aca="false">0.335*Q13</f>
-        <v>1232.31170044899</v>
+        <v>1373.01170044899</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1160,67 +1161,67 @@
       </c>
       <c r="B15" s="1" t="n">
         <f aca="false">B13-B14</f>
-        <v>2005.64</v>
+        <v>2052.19</v>
       </c>
       <c r="C15" s="1" t="n">
         <f aca="false">C13-C14</f>
-        <v>1959.09</v>
+        <v>2052.19</v>
       </c>
       <c r="D15" s="1" t="n">
         <f aca="false">D13-D14</f>
-        <v>1912.54</v>
+        <v>2052.19</v>
       </c>
       <c r="E15" s="1" t="n">
         <f aca="false">E13-E14</f>
-        <v>1865.99</v>
+        <v>2052.19</v>
       </c>
       <c r="F15" s="1" t="n">
         <f aca="false">F13-F14</f>
-        <v>1819.44</v>
+        <v>2052.19</v>
       </c>
       <c r="G15" s="1" t="n">
         <f aca="false">G13-G14</f>
-        <v>1772.89</v>
+        <v>2052.19</v>
       </c>
       <c r="H15" s="1" t="n">
         <f aca="false">H13-H14</f>
-        <v>1835.51704</v>
+        <v>2114.81704</v>
       </c>
       <c r="I15" s="1" t="n">
         <f aca="false">I13-I14</f>
-        <v>1899.14611264</v>
+        <v>2178.44611264</v>
       </c>
       <c r="J15" s="1" t="n">
         <f aca="false">J13-J14</f>
-        <v>1963.79325044224</v>
+        <v>2243.09325044224</v>
       </c>
       <c r="K15" s="1" t="n">
         <f aca="false">K13-K14</f>
-        <v>2029.47474244932</v>
+        <v>2308.77474244932</v>
       </c>
       <c r="L15" s="1" t="n">
         <f aca="false">L13-L14</f>
-        <v>2096.20713832851</v>
+        <v>2375.5071383285</v>
       </c>
       <c r="M15" s="1" t="n">
         <f aca="false">M13-M14</f>
-        <v>2164.00725254176</v>
+        <v>2443.30725254176</v>
       </c>
       <c r="N15" s="1" t="n">
         <f aca="false">N13-N14</f>
-        <v>2232.89216858243</v>
+        <v>2512.19216858243</v>
       </c>
       <c r="O15" s="1" t="n">
         <f aca="false">O13-O14</f>
-        <v>2302.87924327975</v>
+        <v>2582.17924327975</v>
       </c>
       <c r="P15" s="1" t="n">
         <f aca="false">P13-P14</f>
-        <v>2373.98611117222</v>
+        <v>2653.28611117222</v>
       </c>
       <c r="Q15" s="1" t="n">
         <f aca="false">Q13-Q14</f>
-        <v>2446.23068895098</v>
+        <v>2725.53068895098</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1354,62 +1355,62 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="G18" s="1" t="n">
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="H18" s="0" t="n">
         <f aca="false">G18</f>
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="I18" s="0" t="n">
         <f aca="false">H18</f>
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="J18" s="0" t="n">
         <f aca="false">I18</f>
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="K18" s="0" t="n">
         <f aca="false">J18</f>
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="L18" s="0" t="n">
         <f aca="false">K18</f>
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="M18" s="0" t="n">
         <f aca="false">L18</f>
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="N18" s="0" t="n">
         <f aca="false">M18</f>
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="O18" s="0" t="n">
         <f aca="false">N18</f>
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="P18" s="0" t="n">
         <f aca="false">O18</f>
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="Q18" s="0" t="n">
         <f aca="false">P18</f>
-        <v>6000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1418,67 +1419,67 @@
       </c>
       <c r="B19" s="0" t="n">
         <f aca="false">B17+B18</f>
-        <v>21000</v>
+        <v>20000</v>
       </c>
       <c r="C19" s="0" t="n">
         <f aca="false">C17+C18</f>
-        <v>22000</v>
+        <v>20000</v>
       </c>
       <c r="D19" s="0" t="n">
         <f aca="false">D17+D18</f>
-        <v>23000</v>
+        <v>20000</v>
       </c>
       <c r="E19" s="0" t="n">
         <f aca="false">E17+E18</f>
-        <v>24000</v>
+        <v>20000</v>
       </c>
       <c r="F19" s="0" t="n">
         <f aca="false">F17+F18</f>
-        <v>25000</v>
+        <v>20000</v>
       </c>
       <c r="G19" s="1" t="n">
         <f aca="false">G17+G18</f>
-        <v>26000</v>
+        <v>20000</v>
       </c>
       <c r="H19" s="0" t="n">
         <f aca="false">H17+H18</f>
-        <v>26000</v>
+        <v>20000</v>
       </c>
       <c r="I19" s="0" t="n">
         <f aca="false">I17+I18</f>
-        <v>26000</v>
+        <v>20000</v>
       </c>
       <c r="J19" s="0" t="n">
         <f aca="false">J17+J18</f>
-        <v>26000</v>
+        <v>20000</v>
       </c>
       <c r="K19" s="0" t="n">
         <f aca="false">K17+K18</f>
-        <v>26000</v>
+        <v>20000</v>
       </c>
       <c r="L19" s="0" t="n">
         <f aca="false">L17+L18</f>
-        <v>26000</v>
+        <v>20000</v>
       </c>
       <c r="M19" s="0" t="n">
         <f aca="false">M17+M18</f>
-        <v>26000</v>
+        <v>20000</v>
       </c>
       <c r="N19" s="0" t="n">
         <f aca="false">N17+N18</f>
-        <v>26000</v>
+        <v>20000</v>
       </c>
       <c r="O19" s="0" t="n">
         <f aca="false">O17+O18</f>
-        <v>26000</v>
+        <v>20000</v>
       </c>
       <c r="P19" s="0" t="n">
         <f aca="false">P17+P18</f>
-        <v>26000</v>
+        <v>20000</v>
       </c>
       <c r="Q19" s="0" t="n">
         <f aca="false">Q17+Q18</f>
-        <v>26000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1623,67 +1624,67 @@
       </c>
       <c r="B22" s="0" t="n">
         <f aca="false">B15+B8-B20-B21</f>
-        <v>979.545</v>
+        <v>1026.095</v>
       </c>
       <c r="C22" s="0" t="n">
         <f aca="false">C15+C8-C20-C21</f>
-        <v>932.995</v>
+        <v>1026.095</v>
       </c>
       <c r="D22" s="0" t="n">
         <f aca="false">D15+D8-D20-D21</f>
-        <v>886.445</v>
+        <v>1026.095</v>
       </c>
       <c r="E22" s="0" t="n">
         <f aca="false">E15+E8-E20-E21</f>
-        <v>839.895</v>
+        <v>1026.095</v>
       </c>
       <c r="F22" s="0" t="n">
         <f aca="false">F15+F8-F20-F21</f>
-        <v>793.345</v>
+        <v>1026.095</v>
       </c>
       <c r="G22" s="1" t="n">
         <f aca="false">G15+G8-G20-G21</f>
-        <v>746.795</v>
+        <v>1026.095</v>
       </c>
       <c r="H22" s="0" t="n">
         <f aca="false">H15+H8-H20-H21</f>
-        <v>809.422039999999</v>
+        <v>1088.72204</v>
       </c>
       <c r="I22" s="0" t="n">
         <f aca="false">I15+I8-I20-I21</f>
-        <v>873.051112639999</v>
+        <v>1152.35111264</v>
       </c>
       <c r="J22" s="0" t="n">
         <f aca="false">J15+J8-J20-J21</f>
-        <v>937.698250442239</v>
+        <v>1216.99825044224</v>
       </c>
       <c r="K22" s="0" t="n">
         <f aca="false">K15+K8-K20-K21</f>
-        <v>1003.37974244932</v>
+        <v>1282.67974244932</v>
       </c>
       <c r="L22" s="0" t="n">
         <f aca="false">L15+L8-L20-L21</f>
-        <v>1070.11213832851</v>
+        <v>1349.4121383285</v>
       </c>
       <c r="M22" s="0" t="n">
         <f aca="false">M15+M8-M20-M21</f>
-        <v>1137.91225254176</v>
+        <v>1417.21225254176</v>
       </c>
       <c r="N22" s="0" t="n">
         <f aca="false">N15+N8-N20-N21</f>
-        <v>1206.79716858243</v>
+        <v>1486.09716858243</v>
       </c>
       <c r="O22" s="0" t="n">
         <f aca="false">O15+O8-O20-O21</f>
-        <v>1276.78424327975</v>
+        <v>1556.08424327975</v>
       </c>
       <c r="P22" s="0" t="n">
         <f aca="false">P15+P8-P20-P21</f>
-        <v>1347.89111117222</v>
+        <v>1627.19111117222</v>
       </c>
       <c r="Q22" s="0" t="n">
         <f aca="false">Q15+Q8-Q20-Q21</f>
-        <v>1420.13568895098</v>
+        <v>1699.43568895098</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1692,67 +1693,67 @@
       </c>
       <c r="B23" s="0" t="n">
         <f aca="false">0.5*B15</f>
-        <v>1002.82</v>
+        <v>1026.095</v>
       </c>
       <c r="C23" s="0" t="n">
         <f aca="false">0.5*C15</f>
-        <v>979.545</v>
+        <v>1026.095</v>
       </c>
       <c r="D23" s="0" t="n">
         <f aca="false">0.5*D15</f>
-        <v>956.27</v>
+        <v>1026.095</v>
       </c>
       <c r="E23" s="0" t="n">
         <f aca="false">0.5*E15</f>
-        <v>932.995</v>
+        <v>1026.095</v>
       </c>
       <c r="F23" s="0" t="n">
         <f aca="false">0.5*F15</f>
-        <v>909.72</v>
+        <v>1026.095</v>
       </c>
       <c r="G23" s="0" t="n">
         <f aca="false">0.5*G15</f>
-        <v>886.445</v>
+        <v>1026.095</v>
       </c>
       <c r="H23" s="0" t="n">
         <f aca="false">0.5*H15</f>
-        <v>917.75852</v>
+        <v>1057.40852</v>
       </c>
       <c r="I23" s="0" t="n">
         <f aca="false">0.5*I15</f>
-        <v>949.57305632</v>
+        <v>1089.22305632</v>
       </c>
       <c r="J23" s="0" t="n">
         <f aca="false">0.5*J15</f>
-        <v>981.89662522112</v>
+        <v>1121.54662522112</v>
       </c>
       <c r="K23" s="0" t="n">
         <f aca="false">0.5*K15</f>
-        <v>1014.73737122466</v>
+        <v>1154.38737122466</v>
       </c>
       <c r="L23" s="0" t="n">
         <f aca="false">0.5*L15</f>
-        <v>1048.10356916425</v>
+        <v>1187.75356916425</v>
       </c>
       <c r="M23" s="0" t="n">
         <f aca="false">0.5*M15</f>
-        <v>1082.00362627088</v>
+        <v>1221.65362627088</v>
       </c>
       <c r="N23" s="0" t="n">
         <f aca="false">0.5*N15</f>
-        <v>1116.44608429121</v>
+        <v>1256.09608429121</v>
       </c>
       <c r="O23" s="0" t="n">
         <f aca="false">0.5*O15</f>
-        <v>1151.43962163987</v>
+        <v>1291.08962163987</v>
       </c>
       <c r="P23" s="0" t="n">
         <f aca="false">0.5*P15</f>
-        <v>1186.99305558611</v>
+        <v>1326.64305558611</v>
       </c>
       <c r="Q23" s="0" t="n">
         <f aca="false">0.5*Q15</f>
-        <v>1223.11534447549</v>
+        <v>1362.76534447549</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1867,67 +1868,67 @@
       </c>
       <c r="B26" s="0" t="n">
         <f aca="false">B22-B23</f>
-        <v>-23.2749999999999</v>
+        <v>0</v>
       </c>
       <c r="C26" s="0" t="n">
         <f aca="false">C22-C23</f>
-        <v>-46.5500000000001</v>
+        <v>0</v>
       </c>
       <c r="D26" s="0" t="n">
         <f aca="false">D22-D23</f>
-        <v>-69.8250000000003</v>
+        <v>0</v>
       </c>
       <c r="E26" s="0" t="n">
         <f aca="false">E22-E23</f>
-        <v>-93.1000000000004</v>
+        <v>0</v>
       </c>
       <c r="F26" s="0" t="n">
         <f aca="false">F22-F23</f>
-        <v>-116.375</v>
+        <v>0</v>
       </c>
       <c r="G26" s="1" t="n">
         <f aca="false">G22-G23</f>
-        <v>-139.65</v>
+        <v>0</v>
       </c>
       <c r="H26" s="0" t="n">
         <f aca="false">H22-H23</f>
-        <v>-108.33648</v>
+        <v>31.3135199999997</v>
       </c>
       <c r="I26" s="0" t="n">
         <f aca="false">I22-I23</f>
-        <v>-76.5219436800008</v>
+        <v>63.1280563199994</v>
       </c>
       <c r="J26" s="0" t="n">
         <f aca="false">J22-J23</f>
-        <v>-44.1983747788802</v>
+        <v>95.4516252211192</v>
       </c>
       <c r="K26" s="0" t="n">
         <f aca="false">K22-K23</f>
-        <v>-11.3576287753419</v>
+        <v>128.292371224657</v>
       </c>
       <c r="L26" s="0" t="n">
         <f aca="false">L22-L23</f>
-        <v>22.0085691642528</v>
+        <v>161.658569164252</v>
       </c>
       <c r="M26" s="0" t="n">
         <f aca="false">M22-M23</f>
-        <v>55.9086262708802</v>
+        <v>195.55862627088</v>
       </c>
       <c r="N26" s="0" t="n">
         <f aca="false">N22-N23</f>
-        <v>90.3510842912135</v>
+        <v>230.001084291214</v>
       </c>
       <c r="O26" s="0" t="n">
         <f aca="false">O22-O23</f>
-        <v>125.344621639873</v>
+        <v>264.994621639873</v>
       </c>
       <c r="P26" s="0" t="n">
         <f aca="false">P22-P23</f>
-        <v>160.898055586112</v>
+        <v>300.548055586112</v>
       </c>
       <c r="Q26" s="0" t="n">
         <f aca="false">Q22-Q23</f>
-        <v>197.020344475489</v>
+        <v>336.670344475489</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>